<commit_message>
That's a wrap on the report
</commit_message>
<xml_diff>
--- a/Final Report/graphs.xlsx
+++ b/Final Report/graphs.xlsx
@@ -237,11 +237,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="257402528"/>
-        <c:axId val="257398048"/>
+        <c:axId val="293824232"/>
+        <c:axId val="293848424"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="257398048"/>
+        <c:axId val="293848424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -277,7 +277,7 @@
                   <a:tabLst/>
                   <a:defRPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
                     <a:solidFill>
-                      <a:srgbClr val="595959"/>
+                      <a:sysClr val="windowText" lastClr="000000"/>
                     </a:solidFill>
                     <a:latin typeface="Calibri"/>
                     <a:ea typeface=""/>
@@ -287,7 +287,7 @@
                 <a:r>
                   <a:rPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="0" baseline="0">
                     <a:solidFill>
-                      <a:srgbClr val="595959"/>
+                      <a:sysClr val="windowText" lastClr="000000"/>
                     </a:solidFill>
                     <a:uFillTx/>
                     <a:latin typeface="Calibri"/>
@@ -339,7 +339,7 @@
               <a:tabLst/>
               <a:defRPr lang="en-US" sz="1050" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:srgbClr val="595959"/>
+                  <a:sysClr val="windowText" lastClr="000000"/>
                 </a:solidFill>
                 <a:latin typeface="Calibri"/>
                 <a:ea typeface=""/>
@@ -349,12 +349,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="257402528"/>
+        <c:crossAx val="293824232"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="257402528"/>
+        <c:axId val="293824232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -388,9 +388,9 @@
                     <a:spcPts val="0"/>
                   </a:spcAft>
                   <a:tabLst/>
-                  <a:defRPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                  <a:defRPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
                     <a:solidFill>
-                      <a:srgbClr val="595959"/>
+                      <a:sysClr val="windowText" lastClr="000000"/>
                     </a:solidFill>
                     <a:latin typeface="Calibri"/>
                     <a:ea typeface=""/>
@@ -398,9 +398,9 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="0" baseline="0">
+                  <a:rPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="0" baseline="0">
                     <a:solidFill>
-                      <a:srgbClr val="595959"/>
+                      <a:sysClr val="windowText" lastClr="000000"/>
                     </a:solidFill>
                     <a:uFillTx/>
                     <a:latin typeface="Calibri"/>
@@ -452,7 +452,7 @@
               <a:tabLst/>
               <a:defRPr lang="en-US" sz="1050" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:srgbClr val="595959"/>
+                  <a:sysClr val="windowText" lastClr="000000"/>
                 </a:solidFill>
                 <a:latin typeface="Calibri"/>
                 <a:ea typeface=""/>
@@ -462,7 +462,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="257398048"/>
+        <c:crossAx val="293848424"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -721,11 +721,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="258203112"/>
-        <c:axId val="257472632"/>
+        <c:axId val="294395336"/>
+        <c:axId val="293959704"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="258203112"/>
+        <c:axId val="294395336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -751,10 +751,7 @@
                 <a:pPr>
                   <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
+                      <a:sysClr val="windowText" lastClr="000000"/>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
                     <a:ea typeface="+mn-ea"/>
@@ -762,7 +759,11 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-GB" sz="1200"/>
+                  <a:rPr lang="en-GB" sz="1200">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                  </a:rPr>
                   <a:t>Mean Number of cigarettes smoked per day</a:t>
                 </a:r>
               </a:p>
@@ -784,10 +785,7 @@
               <a:pPr>
                 <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
                   <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
+                    <a:sysClr val="windowText" lastClr="000000"/>
                   </a:solidFill>
                   <a:latin typeface="+mn-lt"/>
                   <a:ea typeface="+mn-ea"/>
@@ -819,10 +817,7 @@
             <a:pPr>
               <a:defRPr sz="1050" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
+                  <a:sysClr val="windowText" lastClr="000000"/>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
                 <a:ea typeface="+mn-ea"/>
@@ -832,12 +827,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="257472632"/>
+        <c:crossAx val="293959704"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="257472632"/>
+        <c:axId val="293959704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -863,10 +858,7 @@
                 <a:pPr>
                   <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
+                      <a:sysClr val="windowText" lastClr="000000"/>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
                     <a:ea typeface="+mn-ea"/>
@@ -874,7 +866,11 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-GB" sz="1200"/>
+                  <a:rPr lang="en-GB" sz="1200">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                  </a:rPr>
                   <a:t>% Non-smokers in Network</a:t>
                 </a:r>
               </a:p>
@@ -896,10 +892,7 @@
               <a:pPr>
                 <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
                   <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
+                    <a:sysClr val="windowText" lastClr="000000"/>
                   </a:solidFill>
                   <a:latin typeface="+mn-lt"/>
                   <a:ea typeface="+mn-ea"/>
@@ -931,10 +924,7 @@
             <a:pPr>
               <a:defRPr sz="1050" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
+                  <a:sysClr val="windowText" lastClr="000000"/>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
                 <a:ea typeface="+mn-ea"/>
@@ -944,7 +934,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="258203112"/>
+        <c:crossAx val="294395336"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1151,11 +1141,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="257365776"/>
-        <c:axId val="257298944"/>
+        <c:axId val="294149592"/>
+        <c:axId val="294176040"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="257298944"/>
+        <c:axId val="294176040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1191,7 +1181,7 @@
                   <a:tabLst/>
                   <a:defRPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
                     <a:solidFill>
-                      <a:srgbClr val="595959"/>
+                      <a:sysClr val="windowText" lastClr="000000"/>
                     </a:solidFill>
                     <a:latin typeface="Calibri"/>
                     <a:ea typeface=""/>
@@ -1201,7 +1191,7 @@
                 <a:r>
                   <a:rPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="0" baseline="0">
                     <a:solidFill>
-                      <a:srgbClr val="595959"/>
+                      <a:sysClr val="windowText" lastClr="000000"/>
                     </a:solidFill>
                     <a:uFillTx/>
                     <a:latin typeface="Calibri"/>
@@ -1253,7 +1243,7 @@
               <a:tabLst/>
               <a:defRPr lang="en-US" sz="1050" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:srgbClr val="595959"/>
+                  <a:sysClr val="windowText" lastClr="000000"/>
                 </a:solidFill>
                 <a:latin typeface="Calibri"/>
                 <a:ea typeface=""/>
@@ -1263,12 +1253,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="257365776"/>
+        <c:crossAx val="294149592"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="257365776"/>
+        <c:axId val="294149592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1304,7 +1294,7 @@
                   <a:tabLst/>
                   <a:defRPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
                     <a:solidFill>
-                      <a:srgbClr val="595959"/>
+                      <a:sysClr val="windowText" lastClr="000000"/>
                     </a:solidFill>
                     <a:latin typeface="Calibri"/>
                     <a:ea typeface=""/>
@@ -1314,7 +1304,7 @@
                 <a:r>
                   <a:rPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="0" baseline="0">
                     <a:solidFill>
-                      <a:srgbClr val="595959"/>
+                      <a:sysClr val="windowText" lastClr="000000"/>
                     </a:solidFill>
                     <a:uFillTx/>
                     <a:latin typeface="Calibri"/>
@@ -1366,7 +1356,7 @@
               <a:tabLst/>
               <a:defRPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:srgbClr val="595959"/>
+                  <a:sysClr val="windowText" lastClr="000000"/>
                 </a:solidFill>
                 <a:latin typeface="Calibri"/>
                 <a:ea typeface=""/>
@@ -1376,7 +1366,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="257298944"/>
+        <c:crossAx val="294176040"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1596,11 +1586,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="257460064"/>
-        <c:axId val="257459680"/>
+        <c:axId val="294201632"/>
+        <c:axId val="294218928"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="257459680"/>
+        <c:axId val="294218928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1636,7 +1626,7 @@
                   <a:tabLst/>
                   <a:defRPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
                     <a:solidFill>
-                      <a:srgbClr val="595959"/>
+                      <a:sysClr val="windowText" lastClr="000000"/>
                     </a:solidFill>
                     <a:latin typeface="Calibri"/>
                     <a:ea typeface=""/>
@@ -1646,7 +1636,7 @@
                 <a:r>
                   <a:rPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="0" baseline="0">
                     <a:solidFill>
-                      <a:srgbClr val="595959"/>
+                      <a:sysClr val="windowText" lastClr="000000"/>
                     </a:solidFill>
                     <a:uFillTx/>
                     <a:latin typeface="Calibri"/>
@@ -1698,7 +1688,7 @@
               <a:tabLst/>
               <a:defRPr lang="en-US" sz="1050" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:srgbClr val="595959"/>
+                  <a:sysClr val="windowText" lastClr="000000"/>
                 </a:solidFill>
                 <a:latin typeface="Calibri"/>
                 <a:ea typeface=""/>
@@ -1708,12 +1698,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="257460064"/>
+        <c:crossAx val="294201632"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="257460064"/>
+        <c:axId val="294201632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1749,7 +1739,7 @@
                   <a:tabLst/>
                   <a:defRPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
                     <a:solidFill>
-                      <a:srgbClr val="595959"/>
+                      <a:sysClr val="windowText" lastClr="000000"/>
                     </a:solidFill>
                     <a:latin typeface="Calibri"/>
                     <a:ea typeface=""/>
@@ -1759,7 +1749,7 @@
                 <a:r>
                   <a:rPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="0" baseline="0">
                     <a:solidFill>
-                      <a:srgbClr val="595959"/>
+                      <a:sysClr val="windowText" lastClr="000000"/>
                     </a:solidFill>
                     <a:uFillTx/>
                     <a:latin typeface="Calibri"/>
@@ -1811,7 +1801,7 @@
               <a:tabLst/>
               <a:defRPr lang="en-US" sz="1050" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:srgbClr val="595959"/>
+                  <a:sysClr val="windowText" lastClr="000000"/>
                 </a:solidFill>
                 <a:latin typeface="Calibri"/>
                 <a:ea typeface=""/>
@@ -1821,7 +1811,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="257459680"/>
+        <c:crossAx val="294218928"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1914,6 +1904,450 @@
                 <a:spcPts val="0"/>
               </a:spcAft>
               <a:tabLst/>
+              <a:defRPr lang="en-US" sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="120" baseline="0">
+                <a:solidFill>
+                  <a:srgbClr val="595959"/>
+                </a:solidFill>
+                <a:latin typeface="Calibri"/>
+                <a:ea typeface=""/>
+                <a:cs typeface=""/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="120" baseline="0">
+                <a:solidFill>
+                  <a:srgbClr val="595959"/>
+                </a:solidFill>
+                <a:uFillTx/>
+                <a:latin typeface="Calibri"/>
+                <a:ea typeface=""/>
+                <a:cs typeface=""/>
+              </a:rPr>
+              <a:t>Scale-Free Simulation Runs</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="34925" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="5B9BD5"/>
+              </a:solidFill>
+              <a:prstDash val="solid"/>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:xVal>
+            <c:numRef>
+              <c:f>[1]Sheet1!$I$3:$I$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>73</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>143</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>197</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>271</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>319</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>411</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>507</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>782</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>[1]Sheet1!$L$3:$L$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>27123</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>50359</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>58171</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>92821</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>111926</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>167221</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>184355</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>309941</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="294340608"/>
+        <c:axId val="294340216"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="294340216"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9528" cap="flat">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:prstDash val="solid"/>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr lIns="0" tIns="0" rIns="0" bIns="0"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr marL="0" marR="0" indent="0" algn="ctr" defTabSz="914400" fontAlgn="auto" hangingPunct="1">
+                  <a:lnSpc>
+                    <a:spcPct val="100000"/>
+                  </a:lnSpc>
+                  <a:spcBef>
+                    <a:spcPts val="0"/>
+                  </a:spcBef>
+                  <a:spcAft>
+                    <a:spcPts val="0"/>
+                  </a:spcAft>
+                  <a:tabLst/>
+                  <a:defRPr lang="en-US" sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="Calibri"/>
+                    <a:ea typeface=""/>
+                    <a:cs typeface=""/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="0" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                    <a:uFillTx/>
+                    <a:latin typeface="Calibri"/>
+                    <a:ea typeface=""/>
+                    <a:cs typeface=""/>
+                  </a:rPr>
+                  <a:t>Time Taken (ms)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9528" cap="flat">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:prstDash val="solid"/>
+            <a:round/>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr lIns="0" tIns="0" rIns="0" bIns="0"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr marL="0" marR="0" indent="0" defTabSz="914400" fontAlgn="auto" hangingPunct="1">
+              <a:lnSpc>
+                <a:spcPct val="100000"/>
+              </a:lnSpc>
+              <a:spcBef>
+                <a:spcPts val="0"/>
+              </a:spcBef>
+              <a:spcAft>
+                <a:spcPts val="0"/>
+              </a:spcAft>
+              <a:tabLst/>
+              <a:defRPr lang="en-US" sz="1050" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Calibri"/>
+                <a:ea typeface=""/>
+                <a:cs typeface=""/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="294340608"/>
+        <c:crossesAt val="0"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="294340608"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9528" cap="flat">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:prstDash val="solid"/>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr lIns="0" tIns="0" rIns="0" bIns="0"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr marL="0" marR="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" fontAlgn="auto" hangingPunct="1">
+                  <a:lnSpc>
+                    <a:spcPct val="100000"/>
+                  </a:lnSpc>
+                  <a:spcBef>
+                    <a:spcPts val="0"/>
+                  </a:spcBef>
+                  <a:spcAft>
+                    <a:spcPts val="0"/>
+                  </a:spcAft>
+                  <a:tabLst/>
+                  <a:defRPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="0" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                    <a:uFillTx/>
+                    <a:latin typeface="Calibri"/>
+                    <a:ea typeface=""/>
+                    <a:cs typeface=""/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="0" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                    <a:uFillTx/>
+                    <a:latin typeface="Calibri"/>
+                    <a:ea typeface=""/>
+                    <a:cs typeface=""/>
+                  </a:rPr>
+                  <a:t>Number of Nodes</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9528" cap="flat">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:prstDash val="solid"/>
+            <a:round/>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr lIns="0" tIns="0" rIns="0" bIns="0"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr marL="0" marR="0" indent="0" algn="ctr" defTabSz="914400" fontAlgn="auto" hangingPunct="1">
+              <a:lnSpc>
+                <a:spcPct val="100000"/>
+              </a:lnSpc>
+              <a:spcBef>
+                <a:spcPts val="0"/>
+              </a:spcBef>
+              <a:spcAft>
+                <a:spcPts val="0"/>
+              </a:spcAft>
+              <a:tabLst/>
+              <a:defRPr lang="en-GB" sz="1050" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Calibri"/>
+                <a:ea typeface=""/>
+                <a:cs typeface=""/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="294340216"/>
+        <c:crossesAt val="0"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="FFFFFF"/>
+    </a:solidFill>
+    <a:ln w="9528" cap="flat">
+      <a:noFill/>
+      <a:prstDash val="solid"/>
+      <a:round/>
+    </a:ln>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr lIns="0" tIns="0" rIns="0" bIns="0"/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr marL="0" marR="0" indent="0" defTabSz="914400" fontAlgn="auto" hangingPunct="1">
+        <a:lnSpc>
+          <a:spcPct val="100000"/>
+        </a:lnSpc>
+        <a:spcBef>
+          <a:spcPts val="0"/>
+        </a:spcBef>
+        <a:spcAft>
+          <a:spcPts val="0"/>
+        </a:spcAft>
+        <a:tabLst/>
+        <a:defRPr lang="en-US" sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:latin typeface="Calibri"/>
+          <a:ea typeface=""/>
+          <a:cs typeface=""/>
+        </a:defRPr>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr lIns="0" tIns="0" rIns="0" bIns="0"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr marL="0" marR="0" indent="0" algn="ctr" defTabSz="914400" fontAlgn="auto" hangingPunct="1">
+              <a:lnSpc>
+                <a:spcPct val="100000"/>
+              </a:lnSpc>
+              <a:spcBef>
+                <a:spcPts val="0"/>
+              </a:spcBef>
+              <a:spcAft>
+                <a:spcPts val="0"/>
+              </a:spcAft>
+              <a:tabLst/>
               <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="120" baseline="0">
                 <a:solidFill>
                   <a:srgbClr val="595959"/>
@@ -1963,7 +2397,7 @@
           </c:spPr>
           <c:marker>
             <c:spPr>
-              <a:ln w="34925"/>
+              <a:ln w="44450"/>
             </c:spPr>
           </c:marker>
           <c:xVal>
@@ -2138,11 +2572,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="257825760"/>
-        <c:axId val="257821280"/>
+        <c:axId val="294307768"/>
+        <c:axId val="294307384"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="257821280"/>
+        <c:axId val="294307384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2178,7 +2612,7 @@
                   <a:tabLst/>
                   <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
                     <a:solidFill>
-                      <a:srgbClr val="595959"/>
+                      <a:sysClr val="windowText" lastClr="000000"/>
                     </a:solidFill>
                     <a:latin typeface="Calibri"/>
                     <a:ea typeface=""/>
@@ -2188,7 +2622,7 @@
                 <a:r>
                   <a:rPr lang="en-GB" sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="0" baseline="0">
                     <a:solidFill>
-                      <a:srgbClr val="595959"/>
+                      <a:sysClr val="windowText" lastClr="000000"/>
                     </a:solidFill>
                     <a:uFillTx/>
                     <a:latin typeface="Calibri"/>
@@ -2240,7 +2674,7 @@
               <a:tabLst/>
               <a:defRPr sz="1050" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:srgbClr val="595959"/>
+                  <a:sysClr val="windowText" lastClr="000000"/>
                 </a:solidFill>
                 <a:latin typeface="Calibri"/>
                 <a:ea typeface=""/>
@@ -2250,12 +2684,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="257825760"/>
+        <c:crossAx val="294307768"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="257825760"/>
+        <c:axId val="294307768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2291,7 +2725,7 @@
                   <a:tabLst/>
                   <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
                     <a:solidFill>
-                      <a:srgbClr val="595959"/>
+                      <a:sysClr val="windowText" lastClr="000000"/>
                     </a:solidFill>
                     <a:latin typeface="Calibri"/>
                     <a:ea typeface=""/>
@@ -2301,7 +2735,7 @@
                 <a:r>
                   <a:rPr lang="en-GB" sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="0" baseline="0">
                     <a:solidFill>
-                      <a:srgbClr val="595959"/>
+                      <a:sysClr val="windowText" lastClr="000000"/>
                     </a:solidFill>
                     <a:uFillTx/>
                     <a:latin typeface="Calibri"/>
@@ -2353,7 +2787,7 @@
               <a:tabLst/>
               <a:defRPr sz="1050" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:srgbClr val="595959"/>
+                  <a:sysClr val="windowText" lastClr="000000"/>
                 </a:solidFill>
                 <a:latin typeface="Calibri"/>
                 <a:ea typeface=""/>
@@ -2363,7 +2797,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="257821280"/>
+        <c:crossAx val="294307384"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2425,7 +2859,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -2650,7 +3084,9 @@
           <c:spPr>
             <a:ln w="34925" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent2"/>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -2765,11 +3201,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="257855784"/>
-        <c:axId val="257855392"/>
+        <c:axId val="294338256"/>
+        <c:axId val="294337864"/>
       </c:lineChart>
       <c:valAx>
-        <c:axId val="257855392"/>
+        <c:axId val="294337864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2795,10 +3231,7 @@
                 <a:pPr>
                   <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
+                      <a:sysClr val="windowText" lastClr="000000"/>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
                     <a:ea typeface="+mn-ea"/>
@@ -2806,7 +3239,11 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-GB" sz="1200"/>
+                  <a:rPr lang="en-GB" sz="1200">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                  </a:rPr>
                   <a:t>Ratio / Percentage</a:t>
                 </a:r>
               </a:p>
@@ -2828,10 +3265,7 @@
               <a:pPr>
                 <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
                   <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
+                    <a:sysClr val="windowText" lastClr="000000"/>
                   </a:solidFill>
                   <a:latin typeface="+mn-lt"/>
                   <a:ea typeface="+mn-ea"/>
@@ -2863,10 +3297,7 @@
             <a:pPr>
               <a:defRPr sz="1050" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
+                  <a:sysClr val="windowText" lastClr="000000"/>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
                 <a:ea typeface="+mn-ea"/>
@@ -2876,12 +3307,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="257855784"/>
+        <c:crossAx val="294338256"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="257855784"/>
+        <c:axId val="294338256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2907,10 +3338,7 @@
                 <a:pPr>
                   <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
+                      <a:sysClr val="windowText" lastClr="000000"/>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
                     <a:ea typeface="+mn-ea"/>
@@ -2918,7 +3346,11 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-GB" sz="1200"/>
+                  <a:rPr lang="en-GB" sz="1200">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                  </a:rPr>
                   <a:t>Simulation Number</a:t>
                 </a:r>
               </a:p>
@@ -2940,10 +3372,7 @@
               <a:pPr>
                 <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
                   <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
+                    <a:sysClr val="windowText" lastClr="000000"/>
                   </a:solidFill>
                   <a:latin typeface="+mn-lt"/>
                   <a:ea typeface="+mn-ea"/>
@@ -2974,10 +3403,7 @@
             <a:pPr>
               <a:defRPr sz="1050" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
+                  <a:sysClr val="windowText" lastClr="000000"/>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
                 <a:ea typeface="+mn-ea"/>
@@ -2987,7 +3413,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="257855392"/>
+        <c:crossAx val="294337864"/>
         <c:crossesAt val="0"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3071,7 +3497,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -3263,11 +3689,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="257856568"/>
-        <c:axId val="257856960"/>
+        <c:axId val="294339040"/>
+        <c:axId val="294339432"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="257856568"/>
+        <c:axId val="294339040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3293,10 +3719,7 @@
                 <a:pPr>
                   <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
+                      <a:sysClr val="windowText" lastClr="000000"/>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
                     <a:ea typeface="+mn-ea"/>
@@ -3304,14 +3727,26 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US" sz="1200"/>
+                  <a:rPr lang="en-US" sz="1200">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                  </a:rPr>
                   <a:t>Number</a:t>
                 </a:r>
                 <a:r>
-                  <a:rPr lang="en-US" sz="1200" baseline="0"/>
+                  <a:rPr lang="en-US" sz="1200" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                  </a:rPr>
                   <a:t> of Steps 'Giving up' required to become a non-smoker</a:t>
                 </a:r>
-                <a:endParaRPr lang="en-US" sz="1200"/>
+                <a:endParaRPr lang="en-US" sz="1200">
+                  <a:solidFill>
+                    <a:sysClr val="windowText" lastClr="000000"/>
+                  </a:solidFill>
+                </a:endParaRPr>
               </a:p>
             </c:rich>
           </c:tx>
@@ -3331,10 +3766,7 @@
               <a:pPr>
                 <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
                   <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
+                    <a:sysClr val="windowText" lastClr="000000"/>
                   </a:solidFill>
                   <a:latin typeface="+mn-lt"/>
                   <a:ea typeface="+mn-ea"/>
@@ -3366,10 +3798,7 @@
             <a:pPr>
               <a:defRPr sz="1050" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
+                  <a:sysClr val="windowText" lastClr="000000"/>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
                 <a:ea typeface="+mn-ea"/>
@@ -3379,12 +3808,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="257856960"/>
+        <c:crossAx val="294339432"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="257856960"/>
+        <c:axId val="294339432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3410,10 +3839,7 @@
                 <a:pPr>
                   <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
+                      <a:sysClr val="windowText" lastClr="000000"/>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
                     <a:ea typeface="+mn-ea"/>
@@ -3421,7 +3847,11 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-GB" sz="1200"/>
+                  <a:rPr lang="en-GB" sz="1200">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                  </a:rPr>
                   <a:t>% Non-smokers</a:t>
                 </a:r>
               </a:p>
@@ -3443,10 +3873,7 @@
               <a:pPr>
                 <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
                   <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
+                    <a:sysClr val="windowText" lastClr="000000"/>
                   </a:solidFill>
                   <a:latin typeface="+mn-lt"/>
                   <a:ea typeface="+mn-ea"/>
@@ -3478,10 +3905,7 @@
             <a:pPr>
               <a:defRPr sz="1050" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
+                  <a:sysClr val="windowText" lastClr="000000"/>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
                 <a:ea typeface="+mn-ea"/>
@@ -3491,7 +3915,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="257856568"/>
+        <c:crossAx val="294339040"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3528,449 +3952,6 @@
     <a:p>
       <a:pPr>
         <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="en-US"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr lIns="0" tIns="0" rIns="0" bIns="0"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr marL="0" marR="0" indent="0" algn="ctr" defTabSz="914400" fontAlgn="auto" hangingPunct="1">
-              <a:lnSpc>
-                <a:spcPct val="100000"/>
-              </a:lnSpc>
-              <a:spcBef>
-                <a:spcPts val="0"/>
-              </a:spcBef>
-              <a:spcAft>
-                <a:spcPts val="0"/>
-              </a:spcAft>
-              <a:tabLst/>
-              <a:defRPr lang="en-US" sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="120" baseline="0">
-                <a:solidFill>
-                  <a:srgbClr val="595959"/>
-                </a:solidFill>
-                <a:latin typeface="Calibri"/>
-                <a:ea typeface=""/>
-                <a:cs typeface=""/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US" sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="120" baseline="0">
-                <a:solidFill>
-                  <a:srgbClr val="595959"/>
-                </a:solidFill>
-                <a:uFillTx/>
-                <a:latin typeface="Calibri"/>
-                <a:ea typeface=""/>
-                <a:cs typeface=""/>
-              </a:rPr>
-              <a:t>Scale-Free Simulation Runs</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:layout/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-      </c:spPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:scatterChart>
-        <c:scatterStyle val="lineMarker"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:spPr>
-            <a:ln w="34925" cap="rnd">
-              <a:solidFill>
-                <a:srgbClr val="5B9BD5"/>
-              </a:solidFill>
-              <a:prstDash val="solid"/>
-              <a:round/>
-            </a:ln>
-          </c:spPr>
-          <c:xVal>
-            <c:numRef>
-              <c:f>[1]Sheet1!$I$3:$I$10</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>73</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>143</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>197</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>271</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>319</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>411</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>507</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>782</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>[1]Sheet1!$L$3:$L$10</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>27123</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>50359</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>58171</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>92821</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>111926</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>167221</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>184355</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>309941</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:axId val="257858136"/>
-        <c:axId val="257857744"/>
-      </c:scatterChart>
-      <c:valAx>
-        <c:axId val="257857744"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9528" cap="flat">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:prstDash val="solid"/>
-              <a:round/>
-            </a:ln>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr lIns="0" tIns="0" rIns="0" bIns="0"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr marL="0" marR="0" indent="0" algn="ctr" defTabSz="914400" fontAlgn="auto" hangingPunct="1">
-                  <a:lnSpc>
-                    <a:spcPct val="100000"/>
-                  </a:lnSpc>
-                  <a:spcBef>
-                    <a:spcPts val="0"/>
-                  </a:spcBef>
-                  <a:spcAft>
-                    <a:spcPts val="0"/>
-                  </a:spcAft>
-                  <a:tabLst/>
-                  <a:defRPr lang="en-US" sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
-                    <a:solidFill>
-                      <a:srgbClr val="595959"/>
-                    </a:solidFill>
-                    <a:latin typeface="Calibri"/>
-                    <a:ea typeface=""/>
-                    <a:cs typeface=""/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="0" baseline="0">
-                    <a:solidFill>
-                      <a:srgbClr val="595959"/>
-                    </a:solidFill>
-                    <a:uFillTx/>
-                    <a:latin typeface="Calibri"/>
-                    <a:ea typeface=""/>
-                    <a:cs typeface=""/>
-                  </a:rPr>
-                  <a:t>Time Taken (ms)</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:layout/>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9528" cap="flat">
-            <a:solidFill>
-              <a:schemeClr val="tx1"/>
-            </a:solidFill>
-            <a:prstDash val="solid"/>
-            <a:round/>
-          </a:ln>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr lIns="0" tIns="0" rIns="0" bIns="0"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr marL="0" marR="0" indent="0" defTabSz="914400" fontAlgn="auto" hangingPunct="1">
-              <a:lnSpc>
-                <a:spcPct val="100000"/>
-              </a:lnSpc>
-              <a:spcBef>
-                <a:spcPts val="0"/>
-              </a:spcBef>
-              <a:spcAft>
-                <a:spcPts val="0"/>
-              </a:spcAft>
-              <a:tabLst/>
-              <a:defRPr lang="en-US" sz="1050" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:srgbClr val="595959"/>
-                </a:solidFill>
-                <a:latin typeface="Calibri"/>
-                <a:ea typeface=""/>
-                <a:cs typeface=""/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="257858136"/>
-        <c:crossesAt val="0"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:valAx>
-        <c:axId val="257858136"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9528" cap="flat">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:prstDash val="solid"/>
-              <a:round/>
-            </a:ln>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr lIns="0" tIns="0" rIns="0" bIns="0"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr marL="0" marR="0" indent="0" algn="ctr" defTabSz="914400" fontAlgn="auto" hangingPunct="1">
-                  <a:lnSpc>
-                    <a:spcPct val="100000"/>
-                  </a:lnSpc>
-                  <a:spcBef>
-                    <a:spcPts val="0"/>
-                  </a:spcBef>
-                  <a:spcAft>
-                    <a:spcPts val="0"/>
-                  </a:spcAft>
-                  <a:tabLst/>
-                  <a:defRPr lang="en-US" sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
-                    <a:solidFill>
-                      <a:srgbClr val="595959"/>
-                    </a:solidFill>
-                    <a:latin typeface="Calibri"/>
-                    <a:ea typeface=""/>
-                    <a:cs typeface=""/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="0" baseline="0">
-                    <a:solidFill>
-                      <a:srgbClr val="595959"/>
-                    </a:solidFill>
-                    <a:uFillTx/>
-                    <a:latin typeface="Calibri"/>
-                    <a:ea typeface=""/>
-                    <a:cs typeface=""/>
-                  </a:rPr>
-                  <a:t>Number of Nodes</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:layout/>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9528" cap="flat">
-            <a:solidFill>
-              <a:schemeClr val="tx1"/>
-            </a:solidFill>
-            <a:prstDash val="solid"/>
-            <a:round/>
-          </a:ln>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr lIns="0" tIns="0" rIns="0" bIns="0"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr marL="0" marR="0" indent="0" defTabSz="914400" fontAlgn="auto" hangingPunct="1">
-              <a:lnSpc>
-                <a:spcPct val="100000"/>
-              </a:lnSpc>
-              <a:spcBef>
-                <a:spcPts val="0"/>
-              </a:spcBef>
-              <a:spcAft>
-                <a:spcPts val="0"/>
-              </a:spcAft>
-              <a:tabLst/>
-              <a:defRPr lang="en-US" sz="1050" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:srgbClr val="595959"/>
-                </a:solidFill>
-                <a:latin typeface="Calibri"/>
-                <a:ea typeface=""/>
-                <a:cs typeface=""/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="257857744"/>
-        <c:crossesAt val="0"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-      </c:spPr>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:srgbClr val="FFFFFF"/>
-    </a:solidFill>
-    <a:ln w="9528" cap="flat">
-      <a:noFill/>
-      <a:prstDash val="solid"/>
-      <a:round/>
-    </a:ln>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr lIns="0" tIns="0" rIns="0" bIns="0"/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr marL="0" marR="0" indent="0" defTabSz="914400" fontAlgn="auto" hangingPunct="1">
-        <a:lnSpc>
-          <a:spcPct val="100000"/>
-        </a:lnSpc>
-        <a:spcBef>
-          <a:spcPts val="0"/>
-        </a:spcBef>
-        <a:spcAft>
-          <a:spcPts val="0"/>
-        </a:spcAft>
-        <a:tabLst/>
-        <a:defRPr lang="en-US" sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-          <a:solidFill>
-            <a:srgbClr val="000000"/>
-          </a:solidFill>
-          <a:latin typeface="Calibri"/>
-          <a:ea typeface=""/>
-          <a:cs typeface=""/>
-        </a:defRPr>
       </a:pPr>
       <a:endParaRPr lang="en-US"/>
     </a:p>
@@ -5668,10 +5649,10 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>133353</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>428625</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>114303</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="13424478" cy="7067547"/>
     <xdr:graphicFrame macro="">
@@ -5695,16 +5676,16 @@
   </xdr:oneCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>133350</xdr:colOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>25</xdr:col>
-      <xdr:colOff>142875</xdr:colOff>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>352425</xdr:colOff>
       <xdr:row>37</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -5727,10 +5708,10 @@
   </xdr:twoCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>514350</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="13424474" cy="7058025"/>
     <xdr:graphicFrame macro="">
@@ -5754,10 +5735,10 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>38099</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>48889</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>504824</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>29839</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="13420725" cy="7066286"/>
     <xdr:graphicFrame macro="">
@@ -5781,15 +5762,15 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>609599</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>38099</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>128762</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="13420725" cy="7077075"/>
+    <xdr:ext cx="13432552" cy="7062613"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="10" name="Chart 9"/>
+        <xdr:cNvPr id="2" name="Chart 3"/>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
@@ -5808,9 +5789,36 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>19050</xdr:colOff>
-      <xdr:row>1</xdr:row>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>609599</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>104774</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="13420725" cy="7077075"/>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="10" name="Chart 9"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>0</xdr:row>
       <xdr:rowOff>28574</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="13401675" cy="7077075"/>
@@ -5827,7 +5835,7 @@
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId7"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -5859,39 +5867,12 @@
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId7"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId8"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>426323</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>119237</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="13432552" cy="7062613"/>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 3"/>
-        <xdr:cNvGraphicFramePr>
-          <a:graphicFrameLocks/>
-        </xdr:cNvGraphicFramePr>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId8"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -7228,7 +7209,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AA5" sqref="AA5"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>